<commit_message>
feat/chnage excel file for address
</commit_message>
<xml_diff>
--- a/src/Admin/Order/Component/addressFile.xlsx
+++ b/src/Admin/Order/Component/addressFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soroush\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.hormati\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E6A329-8AD3-4B4A-99FE-0CB0B4701771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D67D4B2-CF31-431A-A731-04143E9CFEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{1C5B3B94-0B5E-4D82-8DFC-666C494CB863}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1C5B3B94-0B5E-4D82-8DFC-666C494CB863}"/>
   </bookViews>
   <sheets>
     <sheet name="تخصیص" sheetId="1" r:id="rId1"/>
@@ -21,22 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>شناسه خرید</t>
   </si>
@@ -53,15 +43,6 @@
     <t>نام تحویل گیرنده</t>
   </si>
   <si>
-    <t>تهران</t>
-  </si>
-  <si>
-    <t>تهران، خیابان نلسون ماندلا، کوچه گلگونه</t>
-  </si>
-  <si>
-    <t>تحویل گیرنده</t>
-  </si>
-  <si>
     <t>IdKharId</t>
   </si>
   <si>
@@ -89,9 +70,6 @@
     <t>PostalCode</t>
   </si>
   <si>
-    <t>ReceiverTel</t>
-  </si>
-  <si>
     <t>ReceiverMobile</t>
   </si>
   <si>
@@ -113,9 +91,6 @@
     <t>آدرس کامل</t>
   </si>
   <si>
-    <t>تلفن تحویل گیرنده</t>
-  </si>
-  <si>
     <t>موبایل تحویل گیرنده</t>
   </si>
   <si>
@@ -147,9 +122,6 @@
   </si>
   <si>
     <t>رشته ای همانند 09121234567</t>
-  </si>
-  <si>
-    <t>رشته ای همانند 0211234567</t>
   </si>
   <si>
     <t>رشته ای همانند کورش آریافر</t>
@@ -177,7 +149,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,12 +159,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -227,21 +193,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -549,7 +516,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -557,110 +524,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C18CC9-03E7-4425-BC4E-8192DA076270}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" customWidth="1"/>
-    <col min="9" max="9" width="31.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="31.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>123</v>
-      </c>
-      <c r="B2">
-        <v>1234</v>
-      </c>
-      <c r="C2">
-        <v>1234</v>
-      </c>
-      <c r="D2">
-        <v>12345</v>
-      </c>
-      <c r="E2">
-        <v>1000</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>123456789</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2">
-        <v>123456789</v>
-      </c>
-      <c r="K2">
-        <v>21111111</v>
-      </c>
-      <c r="L2">
-        <v>9121111111</v>
-      </c>
-      <c r="M2" t="s">
-        <v>7</v>
+      <c r="L1" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -670,171 +592,160 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036863BB-650F-4E4A-A290-F879092B7A8A}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A17" sqref="A17:XFD28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.21875" customWidth="1"/>
-    <col min="2" max="2" width="33.21875" customWidth="1"/>
-    <col min="3" max="3" width="56.33203125" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="56.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="3" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C12" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="B13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>